<commit_message>
Added Test import data.xlsx plus some plots
</commit_message>
<xml_diff>
--- a/test_import_data.xlsx
+++ b/test_import_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="33240" windowHeight="18780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,8 +179,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -188,9 +192,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AI16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AI1"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1917,6 +1925,21 @@
       </c>
       <c r="AI13">
         <v>5.9861385</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35">
+      <c r="M14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35">
+      <c r="M15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35">
+      <c r="M16">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>